<commit_message>
updated for 2023.4 release 27th May 2023
</commit_message>
<xml_diff>
--- a/Modules/MailSentList.xlsx
+++ b/Modules/MailSentList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyoti.raghav\Downloads\GS_Competency Model\GS_Competency Model\Modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843B31B5-2704-4FBE-8966-4E946185D6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDEF1B2-2750-4C4A-8A52-20DC6C44E74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="3860" yWindow="1660" windowWidth="10160" windowHeight="8540" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -33,14 +33,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="457">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="888">
   <x:si>
     <x:t>EmployeeMailId</x:t>
   </x:si>
   <x:si>
+    <x:t>aaron.hubbart@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>aaron.schiel@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>adan.herrera@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>aden.freedman@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -50,9 +56,15 @@
     <x:t>ajay.jagtap@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>alan.delgado@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>alejandro.picado@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>alex.griggs@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>alex.hepburn@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -65,6 +77,18 @@
     <x:t>ali.patel@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>alina.levitchi@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>allison.cruz@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>amir.abbasi@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>andre.cornejo@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>andres.boniche@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -83,6 +107,9 @@
     <x:t>ania.enkhbold@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>anish.ashturkar@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>anjali.payangapaadan@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -92,6 +119,9 @@
     <x:t>aristo.setiawan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>artur.bueno@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ash.karki@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -101,6 +131,15 @@
     <x:t>ashwin.gaddam@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>axel.ramirez@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aziz.virani@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ben.gray@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ben.walthall@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -113,55 +152,139 @@
     <x:t>brandon.hahn@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>breuer.bass@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>brian.burke@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>brian.piret@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>carlos.garduno@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>carlos.viera@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>cesar.arevalo@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>charles.saroka@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>chelsea.dupuy@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>chirag.halani@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>chloe.rosenfeld@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>chris.joseph@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>cristian.ramos@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>curt.lindenberger@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>cynthia.libby@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>daniel.castro@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Daniel.Lerner@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>dave.sorrels@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>david.hernandez@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>dawn.baur@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>deepam.krishnamoorthy@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>denny.chiramel@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>devon.bunyan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>dharak.vasavda@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>diego.turati@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>dina.own@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>don.walker@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>dov.banach@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Drishya.Pillai@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>edwin.tut@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>emily.bernknopf@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>eric.armstrong@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>erick.enciso@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>erik.leaseburg@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>espana.garcia@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>evan.bruns@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ezra.dantowitz@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>faiyaz.shaikh@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fan.zhang@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gary.refka@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>george.hrawi@uipath.com</x:t>
   </x:si>
   <x:si>
-    <x:t>gregory.dikopf@uipath.com</x:t>
+    <x:t>gerasimos.kountouris@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>giannino.lusicic@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gianpier.verutti@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gilberto.garcia@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hector.escobar@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>hunter.mitchell@uipath.com</x:t>
@@ -173,6 +296,12 @@
     <x:t>ibrahim.appiah@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>idan.shani@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Indranil.pal@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ira.monko@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -185,12 +314,18 @@
     <x:t>Jahnavi.Srinadhu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>james.johnson@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>james.lisooey@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>james.reames@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>james.sinocchi@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>james.tan@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -200,33 +335,75 @@
     <x:t>jason.morrison@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jason.webber@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jay.zhang@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>jenny.man@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jeremy.levin@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jesse.turner@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jesus.cuevas@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>johnathan.apuzen@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Johnny.Johnson@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>jonathan.decker@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jonathan.santino@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jorel.medayil@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jorge.rincon@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>jose.gonzalez@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>Joseph.lao@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>joseph.long@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>joseph.rumpza@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>julia.lukovnikova@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>kader.azeez@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>kanika.dubey@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>kati.johnson@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>kellie.mcmillan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kenneth.Braun@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kent.butcher@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>kevin.morath@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -236,33 +413,99 @@
     <x:t>khadir.abdullah@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>kristen.casterline@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kristofer.hoch@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kristopher.kim@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kyle.fenton@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>lacy.simpson@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>leonardo.caldas@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lewis.bell@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>logan.emerson@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>luis.chali@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>luis.colin@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>luis.gonzalez@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>luis.rada@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>luis.serrano@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>luisa.moncaleano@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>luke.gonyea@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>mai.le@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>marcio.bouzon@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>marco.leon@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mario.atallah@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mark.weislow@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>masaki.kumamoto@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>matthew.berube@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>matthew.nguyen@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>max.ott@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Melody.He@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>michael.agarenzo@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>michael.blakely@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>michael.delles@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>michael.lemus@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>michael.leroux@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>michael.mellen@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>michael.taylor@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -275,9 +518,15 @@
     <x:t>mike.fannon@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>mohammad.munir@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>muhammad.ali@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>naji.atallah@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>nathan.dayvault@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -287,36 +536,96 @@
     <x:t>neeharika.thirukkovalluri@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>nelson.wang@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nicole.mervine@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>niraj.banshal@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>noa.olson@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>noah.segal-gould@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>nolyn.croy@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>octavian.popescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>omair.abdul@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>patty.orsini@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>paul.jacobs@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>paul.seda@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>paulo.castillo@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>pavan.venkatrao@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>peter.reischer@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>praveen.ponugoti@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>prerak.patel@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>qadir.ali@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>raamses.gallo@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>rafal.cebula@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rajitha.rupani@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>rajiv.malhotra@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ramesh.pola@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ranjit.jog@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>raul.alonso@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ravi.garg@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>rene.estrada@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>renu.ahluwalia@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rich.buehrle@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>richard.king@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Rigena.Dibra@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>rob.terrio@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -332,24 +641,57 @@
     <x:t>ryan.brown@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ryan.freeman@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sagar.Agrawal@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sam.Cho-Latimer@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>sarah.morrison@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>saurabh.mundhra@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sergio.bentim@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>seth.purkerson@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>shashank.pancharpula@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>sheel.patel@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shiv.saha@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shoaib.ali@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>silvana.schmitt@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>smriti.gupta@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>srujan.gaddam@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>stephen.fowler@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>stephen.lewis@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Stephen.Madigan@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Steven.Bundick@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -359,9 +701,18 @@
     <x:t>sumesh.nair@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>svitlana.dematte@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>tatsuya.emoto@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>teddy.oswari@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tejasvy.narra@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>thomas.steele@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -392,6 +743,24 @@
     <x:t>vincent.lai@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>vinod.bhatt@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vivek.malhotra@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>william.chiu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yael.birin@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yihong.zhuang@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yury.fedorovsky@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>zheng.tan@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -407,39 +776,75 @@
     <x:t>andy.zhu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Antonyne.pushparajan@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ashok.prajapati@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>bingning.han@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>chi.ma@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>cobbie.yang@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>daniel.melfa@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>danny.liao@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eric.yang@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>fai.kwok@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>Hose.Son@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>hyungsoo.kim@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>jaewon.lee@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jessica.kim@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>jim.huang@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jiyoun.kim@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jongman.park@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>junaidy.laures@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>kumyeong.kok@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>marcus.aliwalas@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Michael.Tatti@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>mig.sattwika@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>mike.zhang@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>minoh.kang@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>mohamad.adib@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -449,39 +854,66 @@
     <x:t>Nazhirin.Said@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>pacharapon.bualert@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ryan.zhou@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>sergey.shumilov@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>sky.huang@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tom.lee@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>tomasz.gaczynski@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>valent.anggajaya@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>victor.yu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>waiyee.chin@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>yannick.debruyne@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ying.liu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yongho.gil@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ahmed.gater@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>abhiraj.singh@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>adrian.gorgan@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>adrian.jianu@uipath.com</x:t>
   </x:si>
   <x:si>
-    <x:t>adrian.tudoran@uipath.com</x:t>
-  </x:si>
-  <x:si>
     <x:t>afonso.almeida@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>ana-roxana.ionicioiu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>akanksha.khanna@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>anja.syring@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>alex.popa@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -512,18 +944,36 @@
     <x:t>alexandru-ionel.luca@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>alexey.chistyakov@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>burak.cucu@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>alin.mihalea@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ana-maria.ciocan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>erik.rijken@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>andra.buica@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>andrea.corain@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>andreea.cuculeasa@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>andreea.ghetu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>andreea.pirnac@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>andrei.cristea@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -533,12 +983,39 @@
     <x:t>andrei.stancu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>florentina.antonescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>andu.morie@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>angel.ciobanescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>anna.cocan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>anne-cecile.godin@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>arif.khan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>arkadiusz.soika@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>arkadiusz.starczewski@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>artur.stefanski@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aurelian.sorcaru@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>balwant.raju@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>bar.leiba@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -548,9 +1025,15 @@
     <x:t>beatrice.dobre@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>bennett.llewelyn@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>mandip.gosal@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>norbert.matyas@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>bogdan.gaspar@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -587,6 +1070,9 @@
     <x:t>catalina.cernat@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>sofiane.sahir@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ciprian.sanduleasa@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -596,6 +1082,9 @@
     <x:t>claudiu.sodoleanu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>tjeerd.stap@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>constantin.dumitrascu@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -608,24 +1097,51 @@
     <x:t>cosmin.bucuroiu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>cosmin.duta@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Abdullah.Al-Awlaqi@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>cosmin.ploscaru@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cosmin.simion@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>cristian.belciu@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>cristian.oprescu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>cristina.dumitrescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dan.lica@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>alessandro.rapisarda@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>daniel.ruse@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>daniel.tudoroiu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>daniela.dumitrascu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>darren.cheng@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>diana.mincu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>dion.mes@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>doinita.danuta@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -635,12 +1151,36 @@
     <x:t>dorin.varatic@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>dragos.balauca@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dragos.florescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dragos.leu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dragos.pancescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>eduard.dobre@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>elena.sala@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>emanuel.serban@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>amer.jamaeen@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>erwan.gouyette@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eugen.porumbescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>filip-ioan.zirbo@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -656,10 +1196,16 @@
     <x:t>florin.strugariu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>frederick.harnisch@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>gabriel.chitic@uipath.com</x:t>
   </x:si>
   <x:si>
-    <x:t>george.dumitrascu@uipath.com</x:t>
+    <x:t>gabriel.opran@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gaspare.marino@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>george.lutan@uipath.com</x:t>
@@ -680,12 +1226,33 @@
     <x:t>bogdan.dumitrescu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Horea.Soanca@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ina.mereuta@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gabriela.manea@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>claudiu.tanasescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ion.taran@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ionut.mardare@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ionut.nicula@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ionut-alexandru.pelcea@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>irina.chintoiu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>iustin.nastase@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -698,27 +1265,63 @@
     <x:t>eslam.hassan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>julien.masse@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>julien.vavasseur@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>kamil.makowka@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>kansu.atikler@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>khaldoun.khashan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>khalil.hassim@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>kobi.shaal@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>larisa.povarna@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>laura.mateias@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lavinia.nastase@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>lavinia.toma@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>liviu.leordeanu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>luana.stef@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lucian.enache@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>lucian.ionescu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ludmila.charton@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ludwig.wilhelm@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>lynsey.woodvine@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>madalina.frunza@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>mahir.tuzel@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -728,12 +1331,18 @@
     <x:t>ibrahim.al-ashqar@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>maria.boteanu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>marian.adam@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>marian.petrea@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>marian.platonov@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>mario.sanchez@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -758,6 +1367,9 @@
     <x:t>miguel.melan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ionut.coman@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ionut.macarin@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -770,6 +1382,9 @@
     <x:t>mihai.stiuca@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>mihai.telceanu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>milosz.achcinski@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -782,9 +1397,18 @@
     <x:t>janne.sillanpaa@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Nikita.Biridzhyan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>johnny.chahla@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ninett.panfir@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>magali.philippe@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>marius.avram@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -794,9 +1418,18 @@
     <x:t>ovidiu.pasere@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>paul.gillen@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>paul.placintar@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>paul.punguta@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>philip.ottesen@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>prajwal.shambhu@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -812,6 +1445,15 @@
     <x:t>ramona.fratila@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>rares.ont@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>razvan.dascalu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>razvan.dragomir@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>razvan.iordache@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -824,15 +1466,27 @@
     <x:t>robert.dima@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>robert.waldinger@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>roxana.irinei@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>roxana.unc@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>ryan.harris@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>samuel.eklu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>samuel.orenstenne@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>sanna.koivu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>sebastian.balan@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -845,15 +1499,24 @@
     <x:t>serban.ionut@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>serban.mocanu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>serban.popa@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>sergiu.wittenberger@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>silvia.nan@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>silviu.predan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>simona.dobrescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>normen.luettich@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -863,12 +1526,21 @@
     <x:t>siwar.mezghani@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>snir.pollak@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Robert.Thullner@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>sofiene.jenzri@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>stefan.barabulea@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>roxana.folea@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>sebastian.geisel@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -878,24 +1550,51 @@
     <x:t>tertius.nel@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>stefano.giuliani@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>thomas.endt@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>thomas.moenkemeier@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>tiago.taino@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>tiberiu.niculescu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>umer.kalu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vasilica.corozal@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>victor.aconacena@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>victor.corcodel@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>vlad.anca@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>vlad.chichirau@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>vlad.cioboata@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vlad.ene@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Aashish.mishra@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Abhishek.Tyagi@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>abhyudai.chirumalla@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -908,9 +1607,18 @@
     <x:t>Aman.Sheik@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Amandeep.lall@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ameet.kulkarni@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Amit.Negi@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>amrit.kaur@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Anas.Pv@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -962,6 +1670,9 @@
     <x:t>Bopaiah.ms@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>chaman.shaik@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>chandan.kumar@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -977,9 +1688,15 @@
     <x:t>deepika.kanagaraju@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Dhanraj.Venkatesan@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>dilip.wakdikar@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>diptendu.patra@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Divyojyoti.Sinha@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -992,15 +1709,42 @@
     <x:t>Gaurav.K@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>gayathri.narayanan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>girish.k@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>gourav.kumar@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hari.vignesh@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>himanshu.joshi@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jagdeep.bedi@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>JeevanaPrasad.Koneti@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jyoti.raghav@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kavita.dixit@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>keyul.shah@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>koushik.t@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>krishna.m@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Krishna.Sinha@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1013,15 +1757,36 @@
     <x:t>kumaran.sethu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Lekshmi.R@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Lirikhomba.Ayekpam@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Maaz.Ahmed@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>madhurima.m@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>Mamatha.Kuchipudi@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Manisha.zendekar@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>meera.kannan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Michelle.Henriques@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>minal.gupta@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mohammed.azarudeen@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Monalisa.Maharana@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1043,6 +1808,9 @@
     <x:t>Nikhilesh.Mishra@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>nilekha.repaka@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>oindrila.banerjee@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1055,6 +1823,9 @@
     <x:t>prafful.sharma@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>prasanth.krishnan@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>prashant.shinde@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1064,6 +1835,9 @@
     <x:t>prequiet.loyola@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Priyesh.tiwari@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>rachinder.singh@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1073,6 +1847,9 @@
     <x:t>Rahul.kakkar@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>rahul.kumar@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Rahul.Pasupuleti@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1106,6 +1883,12 @@
     <x:t>Saloni.Juneja@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>sarath.yenigandla@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Sharath.Keshavamurthy@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ShijinMathew.Jacob@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1121,24 +1904,51 @@
     <x:t>Shreya.Shrivastava@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Shreyas.Risodkar@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Siddharth.V@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>sivasankari.s@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>sourav.anand@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Sowmya.Rajan@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>sreejith.ravindran@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Srikirti.raj@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sudheer.kvr@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sugumar.Ramachandran@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>sukannya.jamadar@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>SunilGuptha.Challagandla@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>surabhi.gavali@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Sushanth.Pakki@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Swagatika.Swagatika@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>Swakatha.Suresh@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>uma.pujala@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1157,81 +1967,306 @@
     <x:t>Vishnu.Kothamasu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>bin.ouyang@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tsukasa.matsuyama@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shoji.shigemitsu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>takuji.mizokami@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>yoichi.kawamura@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yosuke.kano@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>kosuke.mogami@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>fumihide.nishimura@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>fumihiro.komoto@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hideaki.fujiwara@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hideaki.usui@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hiroaki.mishima@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hirotaka.takehana@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hirokazu.yatsunami@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>hiroyuki.nozawa@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>hiroshi.kawasaki@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>manabu.nakamura@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yutaro.nakamura@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>manabu.matsudate@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>jun.li@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kazuhiro.kobayashi@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kazuma.kamata@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kazunori.ikeda@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kei.eto@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kiwako.kato@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kosuke.ueno@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kozen.Sai@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>masahiro.harada@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>masaho.toriumi@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mei.li@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>momoe.takada@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>motohiro.asai@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>naoki.ikeda@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>oohan.thet@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>riko.iizuka@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>graham.wong@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>shin.sasaki@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sho.sato@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>so.okuma@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>takashi.shioike@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>takuma.owada@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>teppei.hasegawa@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>xin.hong@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>xueyin.qu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yasuyuki.nishiseki@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>daisuke.kajio@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>hiroo.iwamoto@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yasuhiro.momita@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>kenji.abe2@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yasuhiro.kuranaga@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yuki.tomita@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yuji.miyano@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>marcin.wrobel@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shigenobu.sakurai@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tomoya.nagatsuka@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yasuhiro.natsume@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yoshitaka.nagano@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yuji.katayose@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>daniel.duarte@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>dominic.deandafast@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jose.mansilla@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>kaitlin.auriemma@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>laura.yoon@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>logesh.velu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>moulshree.rangra@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>valerie.gutierrez@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>claudia.radu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>omar.saleh@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Sumit.Sharma@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>harini.satish@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>iago.souza@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>john.dansby@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>bogdan.luca@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>catalin.vilcu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>pantelimon.gulie@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>sonia.memet@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>suzana.neacsu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tetsuji.endo@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>irina.simut@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>ivaylo.bahtchevanov@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>tomohiro.arai@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jayalakshmi.anand@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>leonardo.ruiz@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>vijay.bhaskar@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>aneesh.natarajan@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>ethan.brown@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>kevin.bernstein@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kyle.toillion@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>marcel.lino@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nicoll.crespo@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nouman.arif@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>riti.sharma@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>joshi.kumar@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>kaivin.yong@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>stefano.emodi@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>amit.bhatt@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>emmy.bensoussan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>roksana.dunka-piekarska@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Arun.Kumar@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bhargava.D@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>indrajit.sengupta@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1241,6 +2276,9 @@
     <x:t>cosmin.pandelache@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>toyoki.kajita@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ameht.villalobos@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1253,18 +2291,45 @@
     <x:t>purshotam.rai@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>wenqi.li@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cristina.stan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cristian.ivan@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>teodora.patrascu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>daniel.stanescu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>madalina.popescu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mihai.iorga@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>mihai.gavan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>anna.lee@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>joshua.gregory@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>adam.cone@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ruchi.shah@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>david.santos.gonzalez@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>liana.sarbu@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1274,24 +2339,60 @@
     <x:t>radu.puhalschi@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>xinyu.deng@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>juan.alvarez@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>daniele.passos@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>chirag.surati@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>michael.tomlin@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>toki.akinwamide@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>steven.zhou@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>dalton.russell@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yasuhiro.morita@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>bhanu.chowdavada@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>bhargavi.kammili@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>juan.figueroa@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>harlan.mariaca@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>joan.tacuma@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jose.ordonez@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>miguel.angel@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>alexandre.laffaille@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yidong.wu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>arindam.chatterjee@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1304,18 +2405,93 @@
     <x:t>Yusuke.Kamiyama@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>alin.savu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ayako.watanabe@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>takao.hamamoto@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>ayako.shiraishi@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>hitoshi.ogawa@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>kazuya.fujine@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tanawat.p@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>braulio.cavazos@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sonai.layek@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aaron.collier@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eduardo.cirilli@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>roberto.montufar@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>shiori.osada@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>narcis.szene@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>alexandru.hojda@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cosmin.oanea@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nicu.constantin@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>raisa.tofanel@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>laura.olaru@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>alejandro.moctezuma@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jairo.chaparro@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>andi.sapariuc@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>toshihiko.hayasaka@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yoshinori.ichikawa@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>moises.alvarez@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>david.perez@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nate.bernache@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yusuke.nishida@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Namrata.Lohia@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>michael.moncavage@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1334,10 +2510,37 @@
     <x:t>horia.stefan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>fumiya.donoshita@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mark.kim@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Akshat.Verma@uipath.com</x:t>
   </x:si>
   <x:si>
-    <x:t>daiki.sakai@uipath.com</x:t>
+    <x:t>masatsugu.soga@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>david.mercado@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>juan.carvajalino@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>daniel.londono@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>juan.barajas@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eduardo.sanchez@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jose.aguirre@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>sebastian.munoz@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>aj.saltzberg@uipath.com</x:t>
@@ -1352,18 +2555,45 @@
     <x:t>Nirav.Shah@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yoshifumi.tsuda@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Kapil.Malik@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>alexander.zapata@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>florina.carafa@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yoshihisa.suzuki@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>rohini.nv@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ganesh.kuncha@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eduardo.sencion@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>cleyderman.becerra@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yoshinori.nii@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>Ed.Harriss@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yukiko.yamamoto@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>jorge.avila@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>sheheen.parackal@uipath.com</x:t>
   </x:si>
   <x:si>
@@ -1376,34 +2606,97 @@
     <x:t>uma.kannan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>juan.rendon@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>juan.reyes@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>dikshitha.v@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>juan.rozo@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>shantanu.khaladkar@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>siddartha.narayanan@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>adelyn.xu@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>yair.dines@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>somdipto.ghosh@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>eric.marciano@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>andrea.vasile@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>kalyan.raghavan@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>irina.baragoi@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>dinesh.kumar@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>razvan.clisu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>vetrivelg.g@uipath.com</x:t>
   </x:si>
   <x:si>
     <x:t>Chandra.Keerti@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>sagar.sable@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ramyadevi.t@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>dhruv.patel@uipath.com</x:t>
   </x:si>
   <x:si>
+    <x:t>ionut.vladu@uipath.com</x:t>
+  </x:si>
+  <x:si>
     <x:t>vijay.yadav@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>marko.koskinen@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yusuke.shigemura@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ramkrishna.kadiya@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>yusuke.tsuchida@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>przemyslaw.piecek@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rohit.bachal@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>nicolas.buttin@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eliza.micu@uipath.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>marius.stefan@uipath.com</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1772,7 +3065,7 @@
   <x:dimension ref="A1:A4"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:A2 A2:A850"/>
+      <x:selection activeCell="A2" sqref="A2 A2:XFD1048576 B1:XFD1 A2:A2 A2:A850"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4065,6 +5358,2161 @@
         <x:v>456</x:v>
       </x:c>
     </x:row>
+    <x:row r="458" spans="1:1">
+      <x:c r="A458" s="2" t="s">
+        <x:v>457</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="459" spans="1:1">
+      <x:c r="A459" s="2" t="s">
+        <x:v>458</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="460" spans="1:1">
+      <x:c r="A460" s="2" t="s">
+        <x:v>459</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="461" spans="1:1">
+      <x:c r="A461" s="2" t="s">
+        <x:v>460</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="462" spans="1:1">
+      <x:c r="A462" s="2" t="s">
+        <x:v>461</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="463" spans="1:1">
+      <x:c r="A463" s="2" t="s">
+        <x:v>462</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="464" spans="1:1">
+      <x:c r="A464" s="2" t="s">
+        <x:v>463</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="465" spans="1:1">
+      <x:c r="A465" s="2" t="s">
+        <x:v>464</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="466" spans="1:1">
+      <x:c r="A466" s="2" t="s">
+        <x:v>465</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="467" spans="1:1">
+      <x:c r="A467" s="2" t="s">
+        <x:v>466</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="468" spans="1:1">
+      <x:c r="A468" s="2" t="s">
+        <x:v>467</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="469" spans="1:1">
+      <x:c r="A469" s="2" t="s">
+        <x:v>468</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="470" spans="1:1">
+      <x:c r="A470" s="2" t="s">
+        <x:v>469</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="471" spans="1:1">
+      <x:c r="A471" s="2" t="s">
+        <x:v>470</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="472" spans="1:1">
+      <x:c r="A472" s="2" t="s">
+        <x:v>471</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="473" spans="1:1">
+      <x:c r="A473" s="2" t="s">
+        <x:v>472</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="474" spans="1:1">
+      <x:c r="A474" s="2" t="s">
+        <x:v>473</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="475" spans="1:1">
+      <x:c r="A475" s="2" t="s">
+        <x:v>474</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="476" spans="1:1">
+      <x:c r="A476" s="2" t="s">
+        <x:v>475</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="477" spans="1:1">
+      <x:c r="A477" s="2" t="s">
+        <x:v>476</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="478" spans="1:1">
+      <x:c r="A478" s="2" t="s">
+        <x:v>477</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="479" spans="1:1">
+      <x:c r="A479" s="2" t="s">
+        <x:v>478</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="480" spans="1:1">
+      <x:c r="A480" s="2" t="s">
+        <x:v>479</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="481" spans="1:1">
+      <x:c r="A481" s="2" t="s">
+        <x:v>480</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="482" spans="1:1">
+      <x:c r="A482" s="2" t="s">
+        <x:v>481</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="483" spans="1:1">
+      <x:c r="A483" s="2" t="s">
+        <x:v>482</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="484" spans="1:1">
+      <x:c r="A484" s="2" t="s">
+        <x:v>483</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="485" spans="1:1">
+      <x:c r="A485" s="2" t="s">
+        <x:v>484</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="486" spans="1:1">
+      <x:c r="A486" s="2" t="s">
+        <x:v>485</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="487" spans="1:1">
+      <x:c r="A487" s="2" t="s">
+        <x:v>486</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="488" spans="1:1">
+      <x:c r="A488" s="2" t="s">
+        <x:v>487</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="489" spans="1:1">
+      <x:c r="A489" s="2" t="s">
+        <x:v>488</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="490" spans="1:1">
+      <x:c r="A490" s="2" t="s">
+        <x:v>489</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="491" spans="1:1">
+      <x:c r="A491" s="2" t="s">
+        <x:v>490</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="492" spans="1:1">
+      <x:c r="A492" s="2" t="s">
+        <x:v>491</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="493" spans="1:1">
+      <x:c r="A493" s="2" t="s">
+        <x:v>492</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="494" spans="1:1">
+      <x:c r="A494" s="2" t="s">
+        <x:v>493</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="495" spans="1:1">
+      <x:c r="A495" s="2" t="s">
+        <x:v>494</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="496" spans="1:1">
+      <x:c r="A496" s="2" t="s">
+        <x:v>495</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="497" spans="1:1">
+      <x:c r="A497" s="2" t="s">
+        <x:v>496</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="498" spans="1:1">
+      <x:c r="A498" s="2" t="s">
+        <x:v>497</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="499" spans="1:1">
+      <x:c r="A499" s="2" t="s">
+        <x:v>498</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="500" spans="1:1">
+      <x:c r="A500" s="2" t="s">
+        <x:v>499</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="501" spans="1:1">
+      <x:c r="A501" s="2" t="s">
+        <x:v>500</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="502" spans="1:1">
+      <x:c r="A502" s="2" t="s">
+        <x:v>501</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="503" spans="1:1">
+      <x:c r="A503" s="2" t="s">
+        <x:v>502</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="504" spans="1:1">
+      <x:c r="A504" s="2" t="s">
+        <x:v>503</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="505" spans="1:1">
+      <x:c r="A505" s="2" t="s">
+        <x:v>504</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="506" spans="1:1">
+      <x:c r="A506" s="2" t="s">
+        <x:v>505</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="507" spans="1:1">
+      <x:c r="A507" s="2" t="s">
+        <x:v>506</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="508" spans="1:1">
+      <x:c r="A508" s="2" t="s">
+        <x:v>507</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="509" spans="1:1">
+      <x:c r="A509" s="2" t="s">
+        <x:v>508</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="510" spans="1:1">
+      <x:c r="A510" s="2" t="s">
+        <x:v>509</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="511" spans="1:1">
+      <x:c r="A511" s="2" t="s">
+        <x:v>510</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="512" spans="1:1">
+      <x:c r="A512" s="2" t="s">
+        <x:v>511</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="513" spans="1:1">
+      <x:c r="A513" s="2" t="s">
+        <x:v>512</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="514" spans="1:1">
+      <x:c r="A514" s="2" t="s">
+        <x:v>513</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="515" spans="1:1">
+      <x:c r="A515" s="2" t="s">
+        <x:v>514</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="516" spans="1:1">
+      <x:c r="A516" s="2" t="s">
+        <x:v>515</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="517" spans="1:1">
+      <x:c r="A517" s="2" t="s">
+        <x:v>516</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="518" spans="1:1">
+      <x:c r="A518" s="2" t="s">
+        <x:v>517</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="519" spans="1:1">
+      <x:c r="A519" s="2" t="s">
+        <x:v>518</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="520" spans="1:1">
+      <x:c r="A520" s="2" t="s">
+        <x:v>519</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="521" spans="1:1">
+      <x:c r="A521" s="2" t="s">
+        <x:v>520</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="522" spans="1:1">
+      <x:c r="A522" s="2" t="s">
+        <x:v>521</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="523" spans="1:1">
+      <x:c r="A523" s="2" t="s">
+        <x:v>522</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="524" spans="1:1">
+      <x:c r="A524" s="2" t="s">
+        <x:v>523</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="525" spans="1:1">
+      <x:c r="A525" s="2" t="s">
+        <x:v>524</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="526" spans="1:1">
+      <x:c r="A526" s="2" t="s">
+        <x:v>525</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="527" spans="1:1">
+      <x:c r="A527" s="2" t="s">
+        <x:v>526</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="528" spans="1:1">
+      <x:c r="A528" s="2" t="s">
+        <x:v>527</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="529" spans="1:1">
+      <x:c r="A529" s="2" t="s">
+        <x:v>528</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="530" spans="1:1">
+      <x:c r="A530" s="2" t="s">
+        <x:v>529</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="531" spans="1:1">
+      <x:c r="A531" s="2" t="s">
+        <x:v>530</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="532" spans="1:1">
+      <x:c r="A532" s="2" t="s">
+        <x:v>531</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="533" spans="1:1">
+      <x:c r="A533" s="2" t="s">
+        <x:v>532</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="534" spans="1:1">
+      <x:c r="A534" s="2" t="s">
+        <x:v>533</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="535" spans="1:1">
+      <x:c r="A535" s="2" t="s">
+        <x:v>534</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="536" spans="1:1">
+      <x:c r="A536" s="2" t="s">
+        <x:v>535</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="537" spans="1:1">
+      <x:c r="A537" s="2" t="s">
+        <x:v>536</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="538" spans="1:1">
+      <x:c r="A538" s="2" t="s">
+        <x:v>537</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="539" spans="1:1">
+      <x:c r="A539" s="2" t="s">
+        <x:v>538</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="540" spans="1:1">
+      <x:c r="A540" s="2" t="s">
+        <x:v>539</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="541" spans="1:1">
+      <x:c r="A541" s="2" t="s">
+        <x:v>540</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="542" spans="1:1">
+      <x:c r="A542" s="2" t="s">
+        <x:v>541</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="543" spans="1:1">
+      <x:c r="A543" s="2" t="s">
+        <x:v>542</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="544" spans="1:1">
+      <x:c r="A544" s="2" t="s">
+        <x:v>543</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="545" spans="1:1">
+      <x:c r="A545" s="2" t="s">
+        <x:v>544</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="546" spans="1:1">
+      <x:c r="A546" s="2" t="s">
+        <x:v>545</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="547" spans="1:1">
+      <x:c r="A547" s="2" t="s">
+        <x:v>546</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="548" spans="1:1">
+      <x:c r="A548" s="2" t="s">
+        <x:v>547</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="549" spans="1:1">
+      <x:c r="A549" s="2" t="s">
+        <x:v>548</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="550" spans="1:1">
+      <x:c r="A550" s="2" t="s">
+        <x:v>549</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="551" spans="1:1">
+      <x:c r="A551" s="2" t="s">
+        <x:v>550</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="552" spans="1:1">
+      <x:c r="A552" s="2" t="s">
+        <x:v>551</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="553" spans="1:1">
+      <x:c r="A553" s="2" t="s">
+        <x:v>552</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="554" spans="1:1">
+      <x:c r="A554" s="2" t="s">
+        <x:v>553</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="555" spans="1:1">
+      <x:c r="A555" s="2" t="s">
+        <x:v>554</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="556" spans="1:1">
+      <x:c r="A556" s="2" t="s">
+        <x:v>555</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="557" spans="1:1">
+      <x:c r="A557" s="2" t="s">
+        <x:v>556</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="558" spans="1:1">
+      <x:c r="A558" s="2" t="s">
+        <x:v>557</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="559" spans="1:1">
+      <x:c r="A559" s="2" t="s">
+        <x:v>558</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="560" spans="1:1">
+      <x:c r="A560" s="2" t="s">
+        <x:v>559</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="561" spans="1:1">
+      <x:c r="A561" s="2" t="s">
+        <x:v>560</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="562" spans="1:1">
+      <x:c r="A562" s="2" t="s">
+        <x:v>561</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="563" spans="1:1">
+      <x:c r="A563" s="2" t="s">
+        <x:v>562</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="564" spans="1:1">
+      <x:c r="A564" s="2" t="s">
+        <x:v>563</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="565" spans="1:1">
+      <x:c r="A565" s="2" t="s">
+        <x:v>564</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="566" spans="1:1">
+      <x:c r="A566" s="2" t="s">
+        <x:v>565</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="567" spans="1:1">
+      <x:c r="A567" s="2" t="s">
+        <x:v>566</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="568" spans="1:1">
+      <x:c r="A568" s="2" t="s">
+        <x:v>567</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="569" spans="1:1">
+      <x:c r="A569" s="2" t="s">
+        <x:v>568</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="570" spans="1:1">
+      <x:c r="A570" s="2" t="s">
+        <x:v>569</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="571" spans="1:1">
+      <x:c r="A571" s="2" t="s">
+        <x:v>570</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="572" spans="1:1">
+      <x:c r="A572" s="2" t="s">
+        <x:v>571</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="573" spans="1:1">
+      <x:c r="A573" s="2" t="s">
+        <x:v>572</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="574" spans="1:1">
+      <x:c r="A574" s="2" t="s">
+        <x:v>573</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="575" spans="1:1">
+      <x:c r="A575" s="2" t="s">
+        <x:v>574</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="576" spans="1:1">
+      <x:c r="A576" s="2" t="s">
+        <x:v>575</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="577" spans="1:1">
+      <x:c r="A577" s="2" t="s">
+        <x:v>576</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="578" spans="1:1">
+      <x:c r="A578" s="2" t="s">
+        <x:v>577</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="579" spans="1:1">
+      <x:c r="A579" s="2" t="s">
+        <x:v>578</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="580" spans="1:1">
+      <x:c r="A580" s="2" t="s">
+        <x:v>579</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="581" spans="1:1">
+      <x:c r="A581" s="2" t="s">
+        <x:v>580</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="582" spans="1:1">
+      <x:c r="A582" s="2" t="s">
+        <x:v>581</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="583" spans="1:1">
+      <x:c r="A583" s="2" t="s">
+        <x:v>582</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="584" spans="1:1">
+      <x:c r="A584" s="2" t="s">
+        <x:v>583</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="585" spans="1:1">
+      <x:c r="A585" s="2" t="s">
+        <x:v>584</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="586" spans="1:1">
+      <x:c r="A586" s="2" t="s">
+        <x:v>585</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="587" spans="1:1">
+      <x:c r="A587" s="2" t="s">
+        <x:v>586</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="588" spans="1:1">
+      <x:c r="A588" s="2" t="s">
+        <x:v>587</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="589" spans="1:1">
+      <x:c r="A589" s="2" t="s">
+        <x:v>588</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="590" spans="1:1">
+      <x:c r="A590" s="2" t="s">
+        <x:v>589</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="591" spans="1:1">
+      <x:c r="A591" s="2" t="s">
+        <x:v>590</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="592" spans="1:1">
+      <x:c r="A592" s="2" t="s">
+        <x:v>591</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="593" spans="1:1">
+      <x:c r="A593" s="2" t="s">
+        <x:v>592</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="594" spans="1:1">
+      <x:c r="A594" s="2" t="s">
+        <x:v>593</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="595" spans="1:1">
+      <x:c r="A595" s="2" t="s">
+        <x:v>594</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="596" spans="1:1">
+      <x:c r="A596" s="2" t="s">
+        <x:v>595</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="597" spans="1:1">
+      <x:c r="A597" s="2" t="s">
+        <x:v>596</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="598" spans="1:1">
+      <x:c r="A598" s="2" t="s">
+        <x:v>597</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="599" spans="1:1">
+      <x:c r="A599" s="2" t="s">
+        <x:v>598</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="600" spans="1:1">
+      <x:c r="A600" s="2" t="s">
+        <x:v>599</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="601" spans="1:1">
+      <x:c r="A601" s="2" t="s">
+        <x:v>600</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="602" spans="1:1">
+      <x:c r="A602" s="2" t="s">
+        <x:v>601</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="603" spans="1:1">
+      <x:c r="A603" s="2" t="s">
+        <x:v>602</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="604" spans="1:1">
+      <x:c r="A604" s="2" t="s">
+        <x:v>603</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="605" spans="1:1">
+      <x:c r="A605" s="2" t="s">
+        <x:v>604</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="606" spans="1:1">
+      <x:c r="A606" s="2" t="s">
+        <x:v>605</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="607" spans="1:1">
+      <x:c r="A607" s="2" t="s">
+        <x:v>606</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="608" spans="1:1">
+      <x:c r="A608" s="2" t="s">
+        <x:v>607</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="609" spans="1:1">
+      <x:c r="A609" s="2" t="s">
+        <x:v>608</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="610" spans="1:1">
+      <x:c r="A610" s="2" t="s">
+        <x:v>609</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="611" spans="1:1">
+      <x:c r="A611" s="2" t="s">
+        <x:v>610</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="612" spans="1:1">
+      <x:c r="A612" s="2" t="s">
+        <x:v>611</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="613" spans="1:1">
+      <x:c r="A613" s="2" t="s">
+        <x:v>612</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="614" spans="1:1">
+      <x:c r="A614" s="2" t="s">
+        <x:v>613</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="615" spans="1:1">
+      <x:c r="A615" s="2" t="s">
+        <x:v>614</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="616" spans="1:1">
+      <x:c r="A616" s="2" t="s">
+        <x:v>615</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="617" spans="1:1">
+      <x:c r="A617" s="2" t="s">
+        <x:v>616</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="618" spans="1:1">
+      <x:c r="A618" s="2" t="s">
+        <x:v>617</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="619" spans="1:1">
+      <x:c r="A619" s="2" t="s">
+        <x:v>618</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="620" spans="1:1">
+      <x:c r="A620" s="2" t="s">
+        <x:v>619</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="621" spans="1:1">
+      <x:c r="A621" s="2" t="s">
+        <x:v>620</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="622" spans="1:1">
+      <x:c r="A622" s="2" t="s">
+        <x:v>621</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="623" spans="1:1">
+      <x:c r="A623" s="2" t="s">
+        <x:v>622</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="624" spans="1:1">
+      <x:c r="A624" s="2" t="s">
+        <x:v>623</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="625" spans="1:1">
+      <x:c r="A625" s="2" t="s">
+        <x:v>624</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="626" spans="1:1">
+      <x:c r="A626" s="2" t="s">
+        <x:v>625</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="627" spans="1:1">
+      <x:c r="A627" s="2" t="s">
+        <x:v>626</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="628" spans="1:1">
+      <x:c r="A628" s="2" t="s">
+        <x:v>627</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="629" spans="1:1">
+      <x:c r="A629" s="2" t="s">
+        <x:v>628</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="630" spans="1:1">
+      <x:c r="A630" s="2" t="s">
+        <x:v>629</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="631" spans="1:1">
+      <x:c r="A631" s="2" t="s">
+        <x:v>630</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="632" spans="1:1">
+      <x:c r="A632" s="2" t="s">
+        <x:v>631</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="633" spans="1:1">
+      <x:c r="A633" s="2" t="s">
+        <x:v>632</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="634" spans="1:1">
+      <x:c r="A634" s="2" t="s">
+        <x:v>633</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="635" spans="1:1">
+      <x:c r="A635" s="2" t="s">
+        <x:v>634</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="636" spans="1:1">
+      <x:c r="A636" s="2" t="s">
+        <x:v>635</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="637" spans="1:1">
+      <x:c r="A637" s="2" t="s">
+        <x:v>636</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="638" spans="1:1">
+      <x:c r="A638" s="2" t="s">
+        <x:v>637</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="639" spans="1:1">
+      <x:c r="A639" s="2" t="s">
+        <x:v>638</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="640" spans="1:1">
+      <x:c r="A640" s="2" t="s">
+        <x:v>639</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="641" spans="1:1">
+      <x:c r="A641" s="2" t="s">
+        <x:v>640</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="642" spans="1:1">
+      <x:c r="A642" s="2" t="s">
+        <x:v>641</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="643" spans="1:1">
+      <x:c r="A643" s="2" t="s">
+        <x:v>642</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="644" spans="1:1">
+      <x:c r="A644" s="2" t="s">
+        <x:v>643</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="645" spans="1:1">
+      <x:c r="A645" s="2" t="s">
+        <x:v>644</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="646" spans="1:1">
+      <x:c r="A646" s="2" t="s">
+        <x:v>645</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="647" spans="1:1">
+      <x:c r="A647" s="2" t="s">
+        <x:v>646</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="648" spans="1:1">
+      <x:c r="A648" s="2" t="s">
+        <x:v>647</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="649" spans="1:1">
+      <x:c r="A649" s="2" t="s">
+        <x:v>648</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="650" spans="1:1">
+      <x:c r="A650" s="2" t="s">
+        <x:v>649</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="651" spans="1:1">
+      <x:c r="A651" s="2" t="s">
+        <x:v>650</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="652" spans="1:1">
+      <x:c r="A652" s="2" t="s">
+        <x:v>651</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="653" spans="1:1">
+      <x:c r="A653" s="2" t="s">
+        <x:v>652</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="654" spans="1:1">
+      <x:c r="A654" s="2" t="s">
+        <x:v>653</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="655" spans="1:1">
+      <x:c r="A655" s="2" t="s">
+        <x:v>654</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="656" spans="1:1">
+      <x:c r="A656" s="2" t="s">
+        <x:v>655</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="657" spans="1:1">
+      <x:c r="A657" s="2" t="s">
+        <x:v>656</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="658" spans="1:1">
+      <x:c r="A658" s="2" t="s">
+        <x:v>657</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="659" spans="1:1">
+      <x:c r="A659" s="2" t="s">
+        <x:v>658</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="660" spans="1:1">
+      <x:c r="A660" s="2" t="s">
+        <x:v>659</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="661" spans="1:1">
+      <x:c r="A661" s="2" t="s">
+        <x:v>660</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="662" spans="1:1">
+      <x:c r="A662" s="2" t="s">
+        <x:v>661</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="663" spans="1:1">
+      <x:c r="A663" s="2" t="s">
+        <x:v>662</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="664" spans="1:1">
+      <x:c r="A664" s="2" t="s">
+        <x:v>663</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="665" spans="1:1">
+      <x:c r="A665" s="2" t="s">
+        <x:v>664</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="666" spans="1:1">
+      <x:c r="A666" s="2" t="s">
+        <x:v>665</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="667" spans="1:1">
+      <x:c r="A667" s="2" t="s">
+        <x:v>666</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="668" spans="1:1">
+      <x:c r="A668" s="2" t="s">
+        <x:v>667</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="669" spans="1:1">
+      <x:c r="A669" s="2" t="s">
+        <x:v>668</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="670" spans="1:1">
+      <x:c r="A670" s="2" t="s">
+        <x:v>669</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="671" spans="1:1">
+      <x:c r="A671" s="2" t="s">
+        <x:v>670</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="672" spans="1:1">
+      <x:c r="A672" s="2" t="s">
+        <x:v>671</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="673" spans="1:1">
+      <x:c r="A673" s="2" t="s">
+        <x:v>672</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="674" spans="1:1">
+      <x:c r="A674" s="2" t="s">
+        <x:v>673</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="675" spans="1:1">
+      <x:c r="A675" s="2" t="s">
+        <x:v>674</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="676" spans="1:1">
+      <x:c r="A676" s="2" t="s">
+        <x:v>675</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="677" spans="1:1">
+      <x:c r="A677" s="2" t="s">
+        <x:v>676</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="678" spans="1:1">
+      <x:c r="A678" s="2" t="s">
+        <x:v>677</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="679" spans="1:1">
+      <x:c r="A679" s="2" t="s">
+        <x:v>678</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="680" spans="1:1">
+      <x:c r="A680" s="2" t="s">
+        <x:v>679</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="681" spans="1:1">
+      <x:c r="A681" s="2" t="s">
+        <x:v>680</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="682" spans="1:1">
+      <x:c r="A682" s="2" t="s">
+        <x:v>681</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="683" spans="1:1">
+      <x:c r="A683" s="2" t="s">
+        <x:v>682</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="684" spans="1:1">
+      <x:c r="A684" s="2" t="s">
+        <x:v>683</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="685" spans="1:1">
+      <x:c r="A685" s="2" t="s">
+        <x:v>684</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="686" spans="1:1">
+      <x:c r="A686" s="2" t="s">
+        <x:v>685</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="687" spans="1:1">
+      <x:c r="A687" s="2" t="s">
+        <x:v>686</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="688" spans="1:1">
+      <x:c r="A688" s="2" t="s">
+        <x:v>687</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="689" spans="1:1">
+      <x:c r="A689" s="2" t="s">
+        <x:v>688</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="690" spans="1:1">
+      <x:c r="A690" s="2" t="s">
+        <x:v>689</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="691" spans="1:1">
+      <x:c r="A691" s="2" t="s">
+        <x:v>690</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="692" spans="1:1">
+      <x:c r="A692" s="2" t="s">
+        <x:v>691</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="693" spans="1:1">
+      <x:c r="A693" s="2" t="s">
+        <x:v>692</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="694" spans="1:1">
+      <x:c r="A694" s="2" t="s">
+        <x:v>693</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="695" spans="1:1">
+      <x:c r="A695" s="2" t="s">
+        <x:v>694</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="696" spans="1:1">
+      <x:c r="A696" s="2" t="s">
+        <x:v>695</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="697" spans="1:1">
+      <x:c r="A697" s="2" t="s">
+        <x:v>696</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="698" spans="1:1">
+      <x:c r="A698" s="2" t="s">
+        <x:v>697</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="699" spans="1:1">
+      <x:c r="A699" s="2" t="s">
+        <x:v>698</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="700" spans="1:1">
+      <x:c r="A700" s="2" t="s">
+        <x:v>699</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="701" spans="1:1">
+      <x:c r="A701" s="2" t="s">
+        <x:v>700</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="702" spans="1:1">
+      <x:c r="A702" s="2" t="s">
+        <x:v>701</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="703" spans="1:1">
+      <x:c r="A703" s="2" t="s">
+        <x:v>702</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="704" spans="1:1">
+      <x:c r="A704" s="2" t="s">
+        <x:v>703</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="705" spans="1:1">
+      <x:c r="A705" s="2" t="s">
+        <x:v>704</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="706" spans="1:1">
+      <x:c r="A706" s="2" t="s">
+        <x:v>705</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="707" spans="1:1">
+      <x:c r="A707" s="2" t="s">
+        <x:v>706</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="708" spans="1:1">
+      <x:c r="A708" s="2" t="s">
+        <x:v>707</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="709" spans="1:1">
+      <x:c r="A709" s="2" t="s">
+        <x:v>708</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="710" spans="1:1">
+      <x:c r="A710" s="2" t="s">
+        <x:v>709</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="711" spans="1:1">
+      <x:c r="A711" s="2" t="s">
+        <x:v>710</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="712" spans="1:1">
+      <x:c r="A712" s="2" t="s">
+        <x:v>711</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="713" spans="1:1">
+      <x:c r="A713" s="2" t="s">
+        <x:v>712</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="714" spans="1:1">
+      <x:c r="A714" s="2" t="s">
+        <x:v>713</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="715" spans="1:1">
+      <x:c r="A715" s="2" t="s">
+        <x:v>714</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="716" spans="1:1">
+      <x:c r="A716" s="2" t="s">
+        <x:v>715</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="717" spans="1:1">
+      <x:c r="A717" s="2" t="s">
+        <x:v>716</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="718" spans="1:1">
+      <x:c r="A718" s="2" t="s">
+        <x:v>717</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="719" spans="1:1">
+      <x:c r="A719" s="2" t="s">
+        <x:v>718</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="720" spans="1:1">
+      <x:c r="A720" s="2" t="s">
+        <x:v>719</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="721" spans="1:1">
+      <x:c r="A721" s="2" t="s">
+        <x:v>720</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="722" spans="1:1">
+      <x:c r="A722" s="2" t="s">
+        <x:v>721</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="723" spans="1:1">
+      <x:c r="A723" s="2" t="s">
+        <x:v>722</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="724" spans="1:1">
+      <x:c r="A724" s="2" t="s">
+        <x:v>723</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="725" spans="1:1">
+      <x:c r="A725" s="2" t="s">
+        <x:v>724</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="726" spans="1:1">
+      <x:c r="A726" s="2" t="s">
+        <x:v>725</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="727" spans="1:1">
+      <x:c r="A727" s="2" t="s">
+        <x:v>726</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="728" spans="1:1">
+      <x:c r="A728" s="2" t="s">
+        <x:v>727</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="729" spans="1:1">
+      <x:c r="A729" s="2" t="s">
+        <x:v>728</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="730" spans="1:1">
+      <x:c r="A730" s="2" t="s">
+        <x:v>729</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="731" spans="1:1">
+      <x:c r="A731" s="2" t="s">
+        <x:v>730</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="732" spans="1:1">
+      <x:c r="A732" s="2" t="s">
+        <x:v>731</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="733" spans="1:1">
+      <x:c r="A733" s="2" t="s">
+        <x:v>732</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="734" spans="1:1">
+      <x:c r="A734" s="2" t="s">
+        <x:v>733</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="735" spans="1:1">
+      <x:c r="A735" s="2" t="s">
+        <x:v>734</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="736" spans="1:1">
+      <x:c r="A736" s="2" t="s">
+        <x:v>735</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="737" spans="1:1">
+      <x:c r="A737" s="2" t="s">
+        <x:v>736</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="738" spans="1:1">
+      <x:c r="A738" s="2" t="s">
+        <x:v>737</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="739" spans="1:1">
+      <x:c r="A739" s="2" t="s">
+        <x:v>738</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="740" spans="1:1">
+      <x:c r="A740" s="2" t="s">
+        <x:v>739</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="741" spans="1:1">
+      <x:c r="A741" s="2" t="s">
+        <x:v>740</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="742" spans="1:1">
+      <x:c r="A742" s="2" t="s">
+        <x:v>741</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="743" spans="1:1">
+      <x:c r="A743" s="2" t="s">
+        <x:v>742</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="744" spans="1:1">
+      <x:c r="A744" s="2" t="s">
+        <x:v>743</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="745" spans="1:1">
+      <x:c r="A745" s="2" t="s">
+        <x:v>744</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="746" spans="1:1">
+      <x:c r="A746" s="2" t="s">
+        <x:v>745</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="747" spans="1:1">
+      <x:c r="A747" s="2" t="s">
+        <x:v>746</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="748" spans="1:1">
+      <x:c r="A748" s="2" t="s">
+        <x:v>747</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="749" spans="1:1">
+      <x:c r="A749" s="2" t="s">
+        <x:v>748</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="750" spans="1:1">
+      <x:c r="A750" s="2" t="s">
+        <x:v>749</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="751" spans="1:1">
+      <x:c r="A751" s="2" t="s">
+        <x:v>750</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="752" spans="1:1">
+      <x:c r="A752" s="2" t="s">
+        <x:v>751</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="753" spans="1:1">
+      <x:c r="A753" s="2" t="s">
+        <x:v>752</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="754" spans="1:1">
+      <x:c r="A754" s="2" t="s">
+        <x:v>753</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="755" spans="1:1">
+      <x:c r="A755" s="2" t="s">
+        <x:v>754</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="756" spans="1:1">
+      <x:c r="A756" s="2" t="s">
+        <x:v>755</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="757" spans="1:1">
+      <x:c r="A757" s="2" t="s">
+        <x:v>756</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="758" spans="1:1">
+      <x:c r="A758" s="2" t="s">
+        <x:v>757</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="759" spans="1:1">
+      <x:c r="A759" s="2" t="s">
+        <x:v>758</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="760" spans="1:1">
+      <x:c r="A760" s="2" t="s">
+        <x:v>759</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="761" spans="1:1">
+      <x:c r="A761" s="2" t="s">
+        <x:v>760</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="762" spans="1:1">
+      <x:c r="A762" s="2" t="s">
+        <x:v>761</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="763" spans="1:1">
+      <x:c r="A763" s="2" t="s">
+        <x:v>762</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="764" spans="1:1">
+      <x:c r="A764" s="2" t="s">
+        <x:v>763</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="765" spans="1:1">
+      <x:c r="A765" s="2" t="s">
+        <x:v>764</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="766" spans="1:1">
+      <x:c r="A766" s="2" t="s">
+        <x:v>765</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="767" spans="1:1">
+      <x:c r="A767" s="2" t="s">
+        <x:v>766</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="768" spans="1:1">
+      <x:c r="A768" s="2" t="s">
+        <x:v>767</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="769" spans="1:1">
+      <x:c r="A769" s="2" t="s">
+        <x:v>768</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="770" spans="1:1">
+      <x:c r="A770" s="2" t="s">
+        <x:v>769</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="771" spans="1:1">
+      <x:c r="A771" s="2" t="s">
+        <x:v>770</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="772" spans="1:1">
+      <x:c r="A772" s="2" t="s">
+        <x:v>771</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="773" spans="1:1">
+      <x:c r="A773" s="2" t="s">
+        <x:v>772</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="774" spans="1:1">
+      <x:c r="A774" s="2" t="s">
+        <x:v>773</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="775" spans="1:1">
+      <x:c r="A775" s="2" t="s">
+        <x:v>774</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="776" spans="1:1">
+      <x:c r="A776" s="2" t="s">
+        <x:v>775</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="777" spans="1:1">
+      <x:c r="A777" s="2" t="s">
+        <x:v>776</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="778" spans="1:1">
+      <x:c r="A778" s="2" t="s">
+        <x:v>777</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="779" spans="1:1">
+      <x:c r="A779" s="2" t="s">
+        <x:v>778</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="780" spans="1:1">
+      <x:c r="A780" s="2" t="s">
+        <x:v>779</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="781" spans="1:1">
+      <x:c r="A781" s="2" t="s">
+        <x:v>780</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="782" spans="1:1">
+      <x:c r="A782" s="2" t="s">
+        <x:v>781</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="783" spans="1:1">
+      <x:c r="A783" s="2" t="s">
+        <x:v>782</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="784" spans="1:1">
+      <x:c r="A784" s="2" t="s">
+        <x:v>783</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="785" spans="1:1">
+      <x:c r="A785" s="2" t="s">
+        <x:v>784</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="786" spans="1:1">
+      <x:c r="A786" s="2" t="s">
+        <x:v>785</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="787" spans="1:1">
+      <x:c r="A787" s="2" t="s">
+        <x:v>786</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="788" spans="1:1">
+      <x:c r="A788" s="2" t="s">
+        <x:v>787</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="789" spans="1:1">
+      <x:c r="A789" s="2" t="s">
+        <x:v>788</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="790" spans="1:1">
+      <x:c r="A790" s="2" t="s">
+        <x:v>789</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="791" spans="1:1">
+      <x:c r="A791" s="2" t="s">
+        <x:v>790</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="792" spans="1:1">
+      <x:c r="A792" s="2" t="s">
+        <x:v>791</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="793" spans="1:1">
+      <x:c r="A793" s="2" t="s">
+        <x:v>792</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="794" spans="1:1">
+      <x:c r="A794" s="2" t="s">
+        <x:v>793</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="795" spans="1:1">
+      <x:c r="A795" s="2" t="s">
+        <x:v>794</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="796" spans="1:1">
+      <x:c r="A796" s="2" t="s">
+        <x:v>795</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="797" spans="1:1">
+      <x:c r="A797" s="2" t="s">
+        <x:v>796</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="798" spans="1:1">
+      <x:c r="A798" s="2" t="s">
+        <x:v>797</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="799" spans="1:1">
+      <x:c r="A799" s="2" t="s">
+        <x:v>798</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="800" spans="1:1">
+      <x:c r="A800" s="2" t="s">
+        <x:v>799</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="801" spans="1:1">
+      <x:c r="A801" s="2" t="s">
+        <x:v>800</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="802" spans="1:1">
+      <x:c r="A802" s="2" t="s">
+        <x:v>801</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="803" spans="1:1">
+      <x:c r="A803" s="2" t="s">
+        <x:v>802</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="804" spans="1:1">
+      <x:c r="A804" s="2" t="s">
+        <x:v>803</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="805" spans="1:1">
+      <x:c r="A805" s="2" t="s">
+        <x:v>804</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="806" spans="1:1">
+      <x:c r="A806" s="2" t="s">
+        <x:v>805</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="807" spans="1:1">
+      <x:c r="A807" s="2" t="s">
+        <x:v>806</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="808" spans="1:1">
+      <x:c r="A808" s="2" t="s">
+        <x:v>807</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="809" spans="1:1">
+      <x:c r="A809" s="2" t="s">
+        <x:v>808</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="810" spans="1:1">
+      <x:c r="A810" s="2" t="s">
+        <x:v>809</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="811" spans="1:1">
+      <x:c r="A811" s="2" t="s">
+        <x:v>810</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="812" spans="1:1">
+      <x:c r="A812" s="2" t="s">
+        <x:v>811</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="813" spans="1:1">
+      <x:c r="A813" s="2" t="s">
+        <x:v>812</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="814" spans="1:1">
+      <x:c r="A814" s="2" t="s">
+        <x:v>813</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="815" spans="1:1">
+      <x:c r="A815" s="2" t="s">
+        <x:v>814</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="816" spans="1:1">
+      <x:c r="A816" s="2" t="s">
+        <x:v>815</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="817" spans="1:1">
+      <x:c r="A817" s="2" t="s">
+        <x:v>816</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="818" spans="1:1">
+      <x:c r="A818" s="2" t="s">
+        <x:v>817</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="819" spans="1:1">
+      <x:c r="A819" s="2" t="s">
+        <x:v>818</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="820" spans="1:1">
+      <x:c r="A820" s="2" t="s">
+        <x:v>819</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="821" spans="1:1">
+      <x:c r="A821" s="2" t="s">
+        <x:v>820</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="822" spans="1:1">
+      <x:c r="A822" s="2" t="s">
+        <x:v>821</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="823" spans="1:1">
+      <x:c r="A823" s="2" t="s">
+        <x:v>822</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="824" spans="1:1">
+      <x:c r="A824" s="2" t="s">
+        <x:v>823</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="825" spans="1:1">
+      <x:c r="A825" s="2" t="s">
+        <x:v>824</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="826" spans="1:1">
+      <x:c r="A826" s="2" t="s">
+        <x:v>825</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="827" spans="1:1">
+      <x:c r="A827" s="2" t="s">
+        <x:v>826</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="828" spans="1:1">
+      <x:c r="A828" s="2" t="s">
+        <x:v>827</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="829" spans="1:1">
+      <x:c r="A829" s="2" t="s">
+        <x:v>828</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="830" spans="1:1">
+      <x:c r="A830" s="2" t="s">
+        <x:v>829</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="831" spans="1:1">
+      <x:c r="A831" s="2" t="s">
+        <x:v>830</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="832" spans="1:1">
+      <x:c r="A832" s="2" t="s">
+        <x:v>831</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="833" spans="1:1">
+      <x:c r="A833" s="2" t="s">
+        <x:v>832</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="834" spans="1:1">
+      <x:c r="A834" s="2" t="s">
+        <x:v>833</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="835" spans="1:1">
+      <x:c r="A835" s="2" t="s">
+        <x:v>834</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="836" spans="1:1">
+      <x:c r="A836" s="2" t="s">
+        <x:v>835</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="837" spans="1:1">
+      <x:c r="A837" s="2" t="s">
+        <x:v>836</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="838" spans="1:1">
+      <x:c r="A838" s="2" t="s">
+        <x:v>837</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="839" spans="1:1">
+      <x:c r="A839" s="2" t="s">
+        <x:v>838</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="840" spans="1:1">
+      <x:c r="A840" s="2" t="s">
+        <x:v>839</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="841" spans="1:1">
+      <x:c r="A841" s="2" t="s">
+        <x:v>840</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="842" spans="1:1">
+      <x:c r="A842" s="2" t="s">
+        <x:v>841</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="843" spans="1:1">
+      <x:c r="A843" s="2" t="s">
+        <x:v>842</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="844" spans="1:1">
+      <x:c r="A844" s="2" t="s">
+        <x:v>843</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="845" spans="1:1">
+      <x:c r="A845" s="2" t="s">
+        <x:v>844</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="846" spans="1:1">
+      <x:c r="A846" s="2" t="s">
+        <x:v>845</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="847" spans="1:1">
+      <x:c r="A847" s="2" t="s">
+        <x:v>846</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="848" spans="1:1">
+      <x:c r="A848" s="2" t="s">
+        <x:v>847</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="849" spans="1:1">
+      <x:c r="A849" s="2" t="s">
+        <x:v>848</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="850" spans="1:1">
+      <x:c r="A850" s="2" t="s">
+        <x:v>849</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="851" spans="1:1">
+      <x:c r="A851" s="2" t="s">
+        <x:v>850</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="852" spans="1:1">
+      <x:c r="A852" s="2" t="s">
+        <x:v>851</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="853" spans="1:1">
+      <x:c r="A853" s="2" t="s">
+        <x:v>852</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="854" spans="1:1">
+      <x:c r="A854" s="2" t="s">
+        <x:v>853</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="855" spans="1:1">
+      <x:c r="A855" s="2" t="s">
+        <x:v>854</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="856" spans="1:1">
+      <x:c r="A856" s="2" t="s">
+        <x:v>855</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="857" spans="1:1">
+      <x:c r="A857" s="2" t="s">
+        <x:v>856</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="858" spans="1:1">
+      <x:c r="A858" s="2" t="s">
+        <x:v>857</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="859" spans="1:1">
+      <x:c r="A859" s="2" t="s">
+        <x:v>858</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="860" spans="1:1">
+      <x:c r="A860" s="2" t="s">
+        <x:v>859</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="861" spans="1:1">
+      <x:c r="A861" s="2" t="s">
+        <x:v>860</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="862" spans="1:1">
+      <x:c r="A862" s="2" t="s">
+        <x:v>861</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="863" spans="1:1">
+      <x:c r="A863" s="2" t="s">
+        <x:v>862</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="864" spans="1:1">
+      <x:c r="A864" s="2" t="s">
+        <x:v>863</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="865" spans="1:1">
+      <x:c r="A865" s="2" t="s">
+        <x:v>864</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="866" spans="1:1">
+      <x:c r="A866" s="2" t="s">
+        <x:v>865</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="867" spans="1:1">
+      <x:c r="A867" s="2" t="s">
+        <x:v>866</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="868" spans="1:1">
+      <x:c r="A868" s="2" t="s">
+        <x:v>867</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="869" spans="1:1">
+      <x:c r="A869" s="2" t="s">
+        <x:v>868</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="870" spans="1:1">
+      <x:c r="A870" s="2" t="s">
+        <x:v>869</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="871" spans="1:1">
+      <x:c r="A871" s="2" t="s">
+        <x:v>870</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="872" spans="1:1">
+      <x:c r="A872" s="2" t="s">
+        <x:v>871</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="873" spans="1:1">
+      <x:c r="A873" s="2" t="s">
+        <x:v>872</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="874" spans="1:1">
+      <x:c r="A874" s="2" t="s">
+        <x:v>873</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="875" spans="1:1">
+      <x:c r="A875" s="2" t="s">
+        <x:v>874</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="876" spans="1:1">
+      <x:c r="A876" s="2" t="s">
+        <x:v>875</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="877" spans="1:1">
+      <x:c r="A877" s="2" t="s">
+        <x:v>876</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="878" spans="1:1">
+      <x:c r="A878" s="2" t="s">
+        <x:v>877</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="879" spans="1:1">
+      <x:c r="A879" s="2" t="s">
+        <x:v>878</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="880" spans="1:1">
+      <x:c r="A880" s="2" t="s">
+        <x:v>879</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="881" spans="1:1">
+      <x:c r="A881" s="2" t="s">
+        <x:v>880</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="882" spans="1:1">
+      <x:c r="A882" s="2" t="s">
+        <x:v>881</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="883" spans="1:1">
+      <x:c r="A883" s="2" t="s">
+        <x:v>882</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="884" spans="1:1">
+      <x:c r="A884" s="2" t="s">
+        <x:v>883</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="885" spans="1:1">
+      <x:c r="A885" s="2" t="s">
+        <x:v>884</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="886" spans="1:1">
+      <x:c r="A886" s="2" t="s">
+        <x:v>885</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="887" spans="1:1">
+      <x:c r="A887" s="2" t="s">
+        <x:v>886</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="888" spans="1:1">
+      <x:c r="A888" s="2" t="s">
+        <x:v>887</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>